<commit_message>
Add: Excel - Data Cleaning
</commit_message>
<xml_diff>
--- a/notes/excel/data_cleaning.xlsx
+++ b/notes/excel/data_cleaning.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/github/analytics-portfolio/notes/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C3F4832D-6691-4E80-9CE5-51C600B1F941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E20D31-1B41-F64E-94B6-46B36D96EDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US_Presidents Excel Tutorial Da" sheetId="1" r:id="rId1"/>
+    <sheet name="Clean Version" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Clean Version'!$A$1:$B$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'US_Presidents Excel Tutorial Da'!$A$1:$I$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -24,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="146">
   <si>
     <t>S.No.</t>
   </si>
@@ -443,6 +447,33 @@
   </si>
   <si>
     <t>date updated</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Vice President</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Date Updated</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Aaron Burr</t>
+  </si>
+  <si>
+    <t>George Clinton</t>
+  </si>
+  <si>
+    <t>George M. Dallas</t>
   </si>
 </sst>
 </file>
@@ -451,9 +482,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +621,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -936,12 +974,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1299,16 +1340,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="23.5546875" style="3"/>
+    <col min="7" max="7" width="23.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1375,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1363,7 +1404,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1392,7 +1433,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1421,7 +1462,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1450,7 +1491,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1479,7 +1520,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1508,7 +1549,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1537,7 +1578,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1566,7 +1607,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1595,7 +1636,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1624,7 +1665,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1653,7 +1694,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1682,7 +1723,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1711,7 +1752,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1740,7 +1781,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1769,7 +1810,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1798,7 +1839,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1827,7 +1868,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1856,7 +1897,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1885,7 +1926,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1914,7 +1955,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1943,7 +1984,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1972,7 +2013,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2001,7 +2042,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2030,7 +2071,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2059,7 +2100,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2088,7 +2129,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2117,7 +2158,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2146,7 +2187,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2175,7 +2216,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2204,7 +2245,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2233,7 +2274,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2262,7 +2303,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2291,7 +2332,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2320,7 +2361,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2349,7 +2390,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2378,7 +2419,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2407,7 +2448,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2436,7 +2477,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2465,7 +2506,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2494,7 +2535,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2523,7 +2564,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2552,7 +2593,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2581,7 +2622,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2610,7 +2651,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2639,27 +2680,27 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G47" s="4">
-        <v>395000</v>
+        <v>405000</v>
       </c>
       <c r="H47" s="2">
         <v>44391</v>
@@ -2668,39 +2709,1207 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>44</v>
-      </c>
-      <c r="B48">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="4">
-        <v>405000</v>
-      </c>
-      <c r="H48" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I48" s="2">
-        <v>43862</v>
-      </c>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G48"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0DBB17B-8CF2-AA43-B100-448B5E6AB069}">
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="str">
+        <f>'US_Presidents Excel Tutorial Da'!B1</f>
+        <v>S.No.</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>'US_Presidents Excel Tutorial Da'!B2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D2)</f>
+        <v>Commander-In-Chief  Of The  Continental Army   ( 1775Â€“1783 )</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G2" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>'US_Presidents Excel Tutorial Da'!B3</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D3)</f>
+        <v>1St  Vice President Of The United States</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G3" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>'US_Presidents Excel Tutorial Da'!B4</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D4)</f>
+        <v>2Nd  Vice President Of The United States</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="7">
+        <v>15000</v>
+      </c>
+      <c r="F4" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G4" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>'US_Presidents Excel Tutorial Da'!B5</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D5)</f>
+        <v>5Th  United States Secretary Of State   (1801Â€“1809)</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="7">
+        <v>20000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G5" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f>'US_Presidents Excel Tutorial Da'!B6</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D6)</f>
+        <v>7Th  United States Secretary Of State   (1811Â€“1817)</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7">
+        <v>25000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G6" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>'US_Presidents Excel Tutorial Da'!B7</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D7)</f>
+        <v>8Th  United States Secretary Of State   (1817Â€“1825)</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7">
+        <v>30000</v>
+      </c>
+      <c r="F7" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G7" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>'US_Presidents Excel Tutorial Da'!B8</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D8)</f>
+        <v>U.S. Senator   ( Class 2 )   From  Tennessee   (1823Â€“1825)</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7">
+        <v>35000</v>
+      </c>
+      <c r="F8" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G8" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>'US_Presidents Excel Tutorial Da'!B9</f>
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D9)</f>
+        <v>8Th  Vice President Of The United States</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7">
+        <v>40000</v>
+      </c>
+      <c r="F9" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G9" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f>'US_Presidents Excel Tutorial Da'!B10</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D10)</f>
+        <v>United States Minister To Colombia   (1828Â€“1829)</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7">
+        <v>45000</v>
+      </c>
+      <c r="F10" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G10" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f>'US_Presidents Excel Tutorial Da'!B11</f>
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D11)</f>
+        <v>10Th  Vice President Of The United States</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7">
+        <v>50000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G11" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>'US_Presidents Excel Tutorial Da'!B12</f>
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D12)</f>
+        <v>9Th  Governor Of Tennessee   (1839Â€“1841)</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="7">
+        <v>55000</v>
+      </c>
+      <c r="F12" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G12" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>'US_Presidents Excel Tutorial Da'!B13</f>
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D13)</f>
+        <v>Major General  Of The  1St Infantry Regiment   United States Army   (1846Â€“1849)</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="7">
+        <v>60000</v>
+      </c>
+      <c r="F13" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G13" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f>'US_Presidents Excel Tutorial Da'!B14</f>
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D14)</f>
+        <v>12Th  Vice President Of The United States</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="7">
+        <v>65000</v>
+      </c>
+      <c r="F14" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G14" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f>'US_Presidents Excel Tutorial Da'!B15</f>
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D15)</f>
+        <v>Brigadier General  Of The  9Th Infantry   United States Army   (1847Â€“1848)</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7">
+        <v>75000</v>
+      </c>
+      <c r="F15" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G15" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f>'US_Presidents Excel Tutorial Da'!B16</f>
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D16)</f>
+        <v>United States Minister  To The   Court Of St James'S   (1853Â€“1856)</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="7">
+        <v>85000</v>
+      </c>
+      <c r="F16" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G16" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f>'US_Presidents Excel Tutorial Da'!B17</f>
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D17)</f>
+        <v>U.S. Representative  For  Illinois' 7Th District   (1847Â€“1849)</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="7">
+        <v>95000</v>
+      </c>
+      <c r="F17" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G17" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f>'US_Presidents Excel Tutorial Da'!B18</f>
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D18)</f>
+        <v>16Th  Vice President Of The United States</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="7">
+        <v>105000</v>
+      </c>
+      <c r="F18" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G18" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f>'US_Presidents Excel Tutorial Da'!B19</f>
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D19)</f>
+        <v>Commanding General  Of The U.S. Army   ( 1864Â€“1869 )</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="7">
+        <v>115000</v>
+      </c>
+      <c r="F19" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G19" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f>'US_Presidents Excel Tutorial Da'!B20</f>
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D20)</f>
+        <v>29Th &amp; 32Nd  Governor Of Ohio   (1868Â€“1872 &amp; 1876Â€“1877)</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="7">
+        <v>125000</v>
+      </c>
+      <c r="F20" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G20" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f>'US_Presidents Excel Tutorial Da'!B21</f>
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D21)</f>
+        <v>U.S. Representative  For  Ohio'S 19Th District   (1863Â€“1881)</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="7">
+        <v>135000</v>
+      </c>
+      <c r="F21" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G21" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f>'US_Presidents Excel Tutorial Da'!B22</f>
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D22)</f>
+        <v>20Th  Vice President Of The United States</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="7">
+        <v>145000</v>
+      </c>
+      <c r="F22" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G22" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f>'US_Presidents Excel Tutorial Da'!B23</f>
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D23)</f>
+        <v>28Th  Governor Of New York   (1883Â€“1885)</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="7">
+        <v>155000</v>
+      </c>
+      <c r="F23" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G23" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f>'US_Presidents Excel Tutorial Da'!B24</f>
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D24)</f>
+        <v>U.S. Senator   ( Class 1 )   From  Indiana   (1881Â€“1887)</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="7">
+        <v>165000</v>
+      </c>
+      <c r="F24" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G24" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f>'US_Presidents Excel Tutorial Da'!B25</f>
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D25)</f>
+        <v>22Nd  President Of The United States   (1885Â€“1889)</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="7">
+        <v>175000</v>
+      </c>
+      <c r="F25" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G25" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f>'US_Presidents Excel Tutorial Da'!B26</f>
+        <v>25</v>
+      </c>
+      <c r="B26" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D26)</f>
+        <v>39Th  Governor Of Ohio   (1892Â€“1896)</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="7">
+        <v>185000</v>
+      </c>
+      <c r="F26" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G26" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f>'US_Presidents Excel Tutorial Da'!B27</f>
+        <v>26</v>
+      </c>
+      <c r="B27" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D27)</f>
+        <v>25Th  Vice President Of The United States</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="7">
+        <v>195000</v>
+      </c>
+      <c r="F27" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G27" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f>'US_Presidents Excel Tutorial Da'!B28</f>
+        <v>27</v>
+      </c>
+      <c r="B28" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D28)</f>
+        <v>42Nd  United States Secretary Of War   (1904Â€“1908)</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="7">
+        <v>205000</v>
+      </c>
+      <c r="F28" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G28" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f>'US_Presidents Excel Tutorial Da'!B29</f>
+        <v>28</v>
+      </c>
+      <c r="B29" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D29)</f>
+        <v>34Th  Governor Of New Jersey   (1911Â€“1913)</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="7">
+        <v>225000</v>
+      </c>
+      <c r="F29" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G29" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f>'US_Presidents Excel Tutorial Da'!B30</f>
+        <v>28</v>
+      </c>
+      <c r="B30" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D30)</f>
+        <v>34Th  Governor Of New Jersey   (1911Â€“1913)</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="7">
+        <v>225000</v>
+      </c>
+      <c r="F30" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G30" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f>'US_Presidents Excel Tutorial Da'!B31</f>
+        <v>29</v>
+      </c>
+      <c r="B31" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D31)</f>
+        <v>U.S. Senator   ( Class 3 )   From  Ohio   (1915Â€“1921)</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="7">
+        <v>235000</v>
+      </c>
+      <c r="F31" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G31" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f>'US_Presidents Excel Tutorial Da'!B32</f>
+        <v>30</v>
+      </c>
+      <c r="B32" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D32)</f>
+        <v>29Th  Vice President Of The United States</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="7">
+        <v>245000</v>
+      </c>
+      <c r="F32" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G32" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f>'US_Presidents Excel Tutorial Da'!B33</f>
+        <v>31</v>
+      </c>
+      <c r="B33" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D33)</f>
+        <v>3Rd  United States Secretary Of Commerce   (1921Â€“1928)</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="7">
+        <v>255000</v>
+      </c>
+      <c r="F33" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G33" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f>'US_Presidents Excel Tutorial Da'!B34</f>
+        <v>32</v>
+      </c>
+      <c r="B34" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D34)</f>
+        <v>44Th  Governor Of New York   ( 1929Â€“1932 )</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="7">
+        <v>265000</v>
+      </c>
+      <c r="F34" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G34" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f>'US_Presidents Excel Tutorial Da'!B35</f>
+        <v>33</v>
+      </c>
+      <c r="B35" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D35)</f>
+        <v>34Th  Vice President Of The United States</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="7">
+        <v>275000</v>
+      </c>
+      <c r="F35" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G35" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f>'US_Presidents Excel Tutorial Da'!B36</f>
+        <v>34</v>
+      </c>
+      <c r="B36" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D36)</f>
+        <v>Supreme Allied Commander Europe   ( 1949Â€“1952 )</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="7">
+        <v>285000</v>
+      </c>
+      <c r="F36" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G36" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f>'US_Presidents Excel Tutorial Da'!B37</f>
+        <v>35</v>
+      </c>
+      <c r="B37" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D37)</f>
+        <v>U.S. Senator   ( Class 1 )   From  Massachusetts   (1953Â€“1960)</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="7">
+        <v>295000</v>
+      </c>
+      <c r="F37" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G37" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f>'US_Presidents Excel Tutorial Da'!B38</f>
+        <v>36</v>
+      </c>
+      <c r="B38" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D38)</f>
+        <v>37Th  Vice President Of The United States</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="7">
+        <v>305000</v>
+      </c>
+      <c r="F38" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G38" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f>'US_Presidents Excel Tutorial Da'!B39</f>
+        <v>37</v>
+      </c>
+      <c r="B39" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D39)</f>
+        <v>36Th  Vice President Of The United States   (1953Â€“1961)</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="7">
+        <v>315000</v>
+      </c>
+      <c r="F39" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G39" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f>'US_Presidents Excel Tutorial Da'!B40</f>
+        <v>38</v>
+      </c>
+      <c r="B40" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D40)</f>
+        <v>40Th  Vice President Of The United States</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="7">
+        <v>325000</v>
+      </c>
+      <c r="F40" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G40" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f>'US_Presidents Excel Tutorial Da'!B41</f>
+        <v>39</v>
+      </c>
+      <c r="B41" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D41)</f>
+        <v>76Th  Governor Of Georgia   (1971Â€“1975)</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="7">
+        <v>335000</v>
+      </c>
+      <c r="F41" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G41" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f>'US_Presidents Excel Tutorial Da'!B42</f>
+        <v>40</v>
+      </c>
+      <c r="B42" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D42)</f>
+        <v>33Rd  Governor Of California   ( 1967Â€“1975 )</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="7">
+        <v>345000</v>
+      </c>
+      <c r="F42" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G42" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f>'US_Presidents Excel Tutorial Da'!B43</f>
+        <v>41</v>
+      </c>
+      <c r="B43" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D43)</f>
+        <v>43Rd  Vice President Of The United States</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="7">
+        <v>355000</v>
+      </c>
+      <c r="F43" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G43" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f>'US_Presidents Excel Tutorial Da'!B44</f>
+        <v>42</v>
+      </c>
+      <c r="B44" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D44)</f>
+        <v>40Th &amp; 42Nd  Governor Of Arkansas   (1979Â€“1981 &amp; 1983Â€“1992)</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="7">
+        <v>365000</v>
+      </c>
+      <c r="F44" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G44" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f>'US_Presidents Excel Tutorial Da'!B45</f>
+        <v>43</v>
+      </c>
+      <c r="B45" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D45)</f>
+        <v>46Th  Governor Of Texas   ( 1995Â€“2000 )</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="7">
+        <v>375000</v>
+      </c>
+      <c r="F45" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G45" s="6">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f>'US_Presidents Excel Tutorial Da'!B46</f>
+        <v>44</v>
+      </c>
+      <c r="B46" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D46)</f>
+        <v>U.S. Senator   ( Class 3 )   From  Illinois   ( 2005Â€“2008 )</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E46" s="7">
+        <v>395000</v>
+      </c>
+      <c r="F46" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G46" s="6">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f>'US_Presidents Excel Tutorial Da'!B47</f>
+        <v>45</v>
+      </c>
+      <c r="B47" t="str">
+        <f>PROPER('US_Presidents Excel Tutorial Da'!D47)</f>
+        <v>Chairman Of   The Trump Organization   ( 1971Â€“Present )</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" s="7">
+        <v>405000</v>
+      </c>
+      <c r="F47" s="6">
+        <v>44391</v>
+      </c>
+      <c r="G47" s="6">
+        <v>43862</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B47" xr:uid="{B0DBB17B-8CF2-AA43-B100-448B5E6AB069}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>